<commit_message>
Formato por defecto cuando no se puede parsear la linea
</commit_message>
<xml_diff>
--- a/Horas.xlsx
+++ b/Horas.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>Ano</t>
   </si>
@@ -63,9 +63,6 @@
     <t>TRMProjects</t>
   </si>
   <si>
-    <t>Requirement 8891: HR Mobile - RPA - Mejoras pantalla y exportación a excel</t>
-  </si>
-  <si>
     <t>DFR</t>
   </si>
   <si>
@@ -94,6 +91,18 @@
   </si>
   <si>
     <t>FridayMemo</t>
+  </si>
+  <si>
+    <t>Task 8646: 2 - Report Historic Up´s &amp; Downs</t>
+  </si>
+  <si>
+    <t>Task 8648: 4 - Risk Register (open)</t>
+  </si>
+  <si>
+    <t>Bug 9096: Filtro por proyecto</t>
+  </si>
+  <si>
+    <t>Task 8649: 5 - Risk Register (Open + Closed)</t>
   </si>
 </sst>
 </file>
@@ -170,7 +179,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -179,6 +188,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -460,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -500,34 +510,130 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="4">
         <v>2019</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>7</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="4">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2019</v>
+      </c>
+      <c r="B3" s="4">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4">
+        <v>10</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>2019</v>
+      </c>
+      <c r="B4" s="4">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>2019</v>
+      </c>
+      <c r="B5" s="4">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4">
+        <v>12</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>2019</v>
+      </c>
+      <c r="B6" s="4">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="D6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E3" s="2"/>
+      <c r="G6" s="4">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="https://dev.azure.com/techintprojects/PyCP/_workitems/edit/8646"/>
+    <hyperlink ref="E3" r:id="rId2" display="https://dev.azure.com/techintprojects/PyCP/_workitems/edit/8648"/>
+    <hyperlink ref="E4" r:id="rId3" display="https://dev.azure.com/techintprojects/PyCP/_workitems/edit/8648"/>
+    <hyperlink ref="E5" r:id="rId4" display="https://techintprojects.visualstudio.com/HR/_workitems/edit/9096"/>
+    <hyperlink ref="E6" r:id="rId5" display="https://dev.azure.com/techintprojects/PyCP/_workitems/edit/8649"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -543,12 +649,12 @@
   <sheetData>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
@@ -563,27 +669,27 @@
     </row>
     <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
@@ -593,12 +699,12 @@
     </row>
     <row r="13" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
@@ -608,12 +714,12 @@
     </row>
     <row r="16" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>